<commit_message>
tracking cost evaluationg done --- but terrain variablity is not good enough
</commit_message>
<xml_diff>
--- a/RefMotion/Knitro/flat_ref/stats.xlsx
+++ b/RefMotion/Knitro/flat_ref/stats.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="50">
-  <si>
-    <t>1 Step LookAhaed</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="49">
+  <si>
+    <t>2 Step LookAhaed</t>
   </si>
   <si>
     <t>0 Trial</t>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Terminal Z</t>
-  </si>
-  <si>
-    <t>2 Step LookAhaed</t>
   </si>
   <si>
     <t>3 Step LookAhaed</t>
@@ -495,54 +492,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE40"/>
+  <dimension ref="G1:BE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:57">
-      <c r="A1" t="s">
+    <row r="1" spans="7:57">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>44</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AK1" t="s">
         <v>45</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AQ1" t="s">
         <v>46</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BC1" t="s">
         <v>48</v>
       </c>
-      <c r="BC1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:57">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="3" spans="7:57">
       <c r="G3" t="s">
         <v>1</v>
       </c>
@@ -625,2886 +610,2730 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:57">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>5.05769</v>
-      </c>
-      <c r="C4">
-        <v>5.4699</v>
-      </c>
+    <row r="4" spans="7:57">
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4">
-        <v>10.73919</v>
+        <v>16.94139</v>
       </c>
       <c r="I4">
-        <v>11</v>
+        <v>17.271</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
       </c>
       <c r="N4">
-        <v>20.59757</v>
+        <v>20.93394</v>
       </c>
       <c r="O4">
-        <v>20.954</v>
+        <v>21.378</v>
       </c>
       <c r="S4" t="s">
         <v>4</v>
       </c>
       <c r="T4">
-        <v>51.1792</v>
+        <v>24.38121</v>
       </c>
       <c r="U4">
-        <v>51.488</v>
+        <v>24.665</v>
       </c>
       <c r="Y4" t="s">
         <v>4</v>
       </c>
       <c r="Z4">
-        <v>38.63456</v>
+        <v>31.14274</v>
       </c>
       <c r="AA4">
-        <v>39.01</v>
+        <v>31.575</v>
       </c>
       <c r="AE4" t="s">
         <v>4</v>
       </c>
       <c r="AF4">
-        <v>18.917</v>
+        <v>74.39066</v>
       </c>
       <c r="AG4">
-        <v>19.21</v>
+        <v>74.63800000000001</v>
       </c>
       <c r="AK4" t="s">
         <v>4</v>
       </c>
       <c r="AL4">
-        <v>77.80722</v>
+        <v>69.51508</v>
       </c>
       <c r="AM4">
-        <v>78.08</v>
+        <v>69.81399999999999</v>
       </c>
       <c r="AQ4" t="s">
         <v>4</v>
       </c>
       <c r="AR4">
-        <v>45.38794</v>
+        <v>75.30463</v>
       </c>
       <c r="AS4">
-        <v>45.453</v>
+        <v>75.547</v>
       </c>
       <c r="AW4" t="s">
         <v>4</v>
       </c>
       <c r="AX4">
-        <v>229.85045</v>
+        <v>91.81538</v>
       </c>
       <c r="AY4">
-        <v>229.79</v>
+        <v>91.90000000000001</v>
       </c>
       <c r="BC4" t="s">
         <v>4</v>
       </c>
       <c r="BD4">
-        <v>167.40068</v>
+        <v>57.09493</v>
       </c>
       <c r="BE4">
-        <v>166.97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:57">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>3.26074</v>
-      </c>
-      <c r="C5">
-        <v>3.453</v>
-      </c>
+        <v>57.164</v>
+      </c>
+    </row>
+    <row r="5" spans="7:57">
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5">
-        <v>1.37036</v>
+        <v>0.5061600000000001</v>
       </c>
       <c r="I5">
-        <v>1.6095</v>
+        <v>0.747</v>
       </c>
       <c r="M5" t="s">
         <v>5</v>
       </c>
       <c r="N5">
-        <v>0.96933</v>
+        <v>2.0241</v>
       </c>
       <c r="O5">
-        <v>1.1953</v>
+        <v>2.2706</v>
       </c>
       <c r="S5" t="s">
         <v>5</v>
       </c>
       <c r="T5">
-        <v>11.99986</v>
+        <v>6.50721</v>
       </c>
       <c r="U5">
-        <v>12.131</v>
+        <v>6.7261</v>
       </c>
       <c r="Y5" t="s">
         <v>5</v>
       </c>
       <c r="Z5">
-        <v>6.35179</v>
+        <v>19.03317</v>
       </c>
       <c r="AA5">
-        <v>6.5451</v>
+        <v>19.197</v>
       </c>
       <c r="AE5" t="s">
         <v>5</v>
       </c>
       <c r="AF5">
-        <v>13.40506</v>
+        <v>15.38829</v>
       </c>
       <c r="AG5">
-        <v>13.59</v>
+        <v>15.575</v>
       </c>
       <c r="AK5" t="s">
         <v>5</v>
       </c>
       <c r="AL5">
-        <v>26.33991</v>
+        <v>39.89273</v>
       </c>
       <c r="AM5">
-        <v>26.523</v>
+        <v>40.078</v>
       </c>
       <c r="AQ5" t="s">
         <v>5</v>
       </c>
       <c r="AR5">
-        <v>30.37657</v>
+        <v>52.42473</v>
       </c>
       <c r="AS5">
-        <v>30.503</v>
+        <v>52.659</v>
       </c>
       <c r="AW5" t="s">
         <v>5</v>
       </c>
       <c r="AX5">
-        <v>10.75213</v>
+        <v>60.84423</v>
       </c>
       <c r="AY5">
-        <v>10.906</v>
+        <v>60.986</v>
       </c>
       <c r="BC5" t="s">
         <v>5</v>
       </c>
       <c r="BD5">
-        <v>73.07053000000001</v>
+        <v>57.20883</v>
       </c>
       <c r="BE5">
-        <v>72.82299999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:57">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
+        <v>57.355</v>
+      </c>
+    </row>
+    <row r="6" spans="7:57">
       <c r="G6" t="s">
         <v>6</v>
       </c>
       <c r="H6">
-        <v>0.46883</v>
+        <v>0.50822</v>
       </c>
       <c r="I6">
-        <v>0.7062</v>
+        <v>0.7625999999999999</v>
       </c>
       <c r="M6" t="s">
         <v>6</v>
       </c>
       <c r="N6">
-        <v>1.2319</v>
+        <v>1.32984</v>
       </c>
       <c r="O6">
-        <v>1.4567</v>
+        <v>1.5785</v>
       </c>
       <c r="S6" t="s">
         <v>6</v>
       </c>
       <c r="T6">
-        <v>1.50243</v>
+        <v>1.4374</v>
       </c>
       <c r="U6">
-        <v>1.7137</v>
+        <v>1.6565</v>
       </c>
       <c r="Y6" t="s">
         <v>6</v>
       </c>
       <c r="Z6">
-        <v>2.54774</v>
+        <v>2.36994</v>
       </c>
       <c r="AA6">
-        <v>2.7446</v>
+        <v>2.5854</v>
       </c>
       <c r="AE6" t="s">
         <v>6</v>
       </c>
       <c r="AF6">
-        <v>2.76701</v>
+        <v>4.21291</v>
       </c>
       <c r="AG6">
-        <v>2.9539</v>
+        <v>4.4152</v>
       </c>
       <c r="AK6" t="s">
         <v>6</v>
       </c>
       <c r="AL6">
-        <v>3.54296</v>
+        <v>3.4376</v>
       </c>
       <c r="AM6">
-        <v>3.7222</v>
+        <v>3.6183</v>
       </c>
       <c r="AQ6" t="s">
         <v>6</v>
       </c>
       <c r="AR6">
-        <v>5.30926</v>
+        <v>7.75726</v>
       </c>
       <c r="AS6">
-        <v>5.5225</v>
+        <v>7.9286</v>
       </c>
       <c r="AW6" t="s">
         <v>6</v>
       </c>
       <c r="AX6">
-        <v>5.36998</v>
+        <v>4.89331</v>
       </c>
       <c r="AY6">
-        <v>5.596</v>
+        <v>5.058</v>
       </c>
       <c r="BC6" t="s">
         <v>6</v>
       </c>
       <c r="BD6">
-        <v>7.85591</v>
+        <v>5.46719</v>
       </c>
       <c r="BE6">
-        <v>7.9271</v>
-      </c>
-    </row>
-    <row r="7" spans="1:57">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
+        <v>5.6161</v>
+      </c>
+    </row>
+    <row r="7" spans="7:57">
       <c r="G7" t="s">
         <v>7</v>
       </c>
       <c r="H7">
-        <v>0.57798</v>
+        <v>0.34891</v>
       </c>
       <c r="I7">
-        <v>0.8147</v>
+        <v>0.6034</v>
       </c>
       <c r="M7" t="s">
         <v>7</v>
       </c>
       <c r="N7">
-        <v>0.87819</v>
+        <v>0.98348</v>
       </c>
       <c r="O7">
-        <v>1.104</v>
+        <v>1.2355</v>
       </c>
       <c r="S7" t="s">
         <v>7</v>
       </c>
       <c r="T7">
-        <v>1.4309</v>
+        <v>1.65039</v>
       </c>
       <c r="U7">
-        <v>1.6354</v>
+        <v>1.8701</v>
       </c>
       <c r="Y7" t="s">
         <v>7</v>
       </c>
       <c r="Z7">
-        <v>2.17524</v>
+        <v>2.45213</v>
       </c>
       <c r="AA7">
-        <v>2.3795</v>
+        <v>2.6524</v>
       </c>
       <c r="AE7" t="s">
         <v>7</v>
       </c>
       <c r="AF7">
-        <v>2.78295</v>
+        <v>2.94</v>
       </c>
       <c r="AG7">
-        <v>2.9764</v>
+        <v>3.1659</v>
       </c>
       <c r="AK7" t="s">
         <v>7</v>
       </c>
       <c r="AL7">
-        <v>3.32444</v>
+        <v>3.03178</v>
       </c>
       <c r="AM7">
-        <v>3.4979</v>
+        <v>3.2217</v>
       </c>
       <c r="AQ7" t="s">
         <v>7</v>
       </c>
       <c r="AR7">
-        <v>3.95998</v>
+        <v>4.23896</v>
       </c>
       <c r="AS7">
-        <v>4.1165</v>
+        <v>4.4445</v>
       </c>
       <c r="AW7" t="s">
         <v>7</v>
       </c>
       <c r="AX7">
-        <v>4.55017</v>
+        <v>4.78378</v>
       </c>
       <c r="AY7">
-        <v>4.7037</v>
+        <v>5.0169</v>
       </c>
       <c r="BC7" t="s">
         <v>7</v>
       </c>
       <c r="BD7">
-        <v>7.7513</v>
+        <v>5.00562</v>
       </c>
       <c r="BE7">
-        <v>7.5901</v>
-      </c>
-    </row>
-    <row r="8" spans="1:57">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
+        <v>5.1597</v>
+      </c>
+    </row>
+    <row r="8" spans="7:57">
       <c r="G8" t="s">
         <v>8</v>
       </c>
       <c r="H8">
-        <v>0.40793</v>
+        <v>0.34599</v>
       </c>
       <c r="I8">
-        <v>0.6468</v>
+        <v>0.6004</v>
       </c>
       <c r="M8" t="s">
         <v>8</v>
       </c>
       <c r="N8">
-        <v>0.80884</v>
+        <v>0.54287</v>
       </c>
       <c r="O8">
-        <v>1.0597</v>
+        <v>0.7739</v>
       </c>
       <c r="S8" t="s">
         <v>8</v>
       </c>
       <c r="T8">
-        <v>1.66392</v>
+        <v>1.59943</v>
       </c>
       <c r="U8">
-        <v>1.857</v>
+        <v>1.819</v>
       </c>
       <c r="Y8" t="s">
         <v>8</v>
       </c>
       <c r="Z8">
-        <v>2.29552</v>
+        <v>2.47947</v>
       </c>
       <c r="AA8">
-        <v>2.5002</v>
+        <v>2.7223</v>
       </c>
       <c r="AE8" t="s">
         <v>8</v>
       </c>
       <c r="AF8">
-        <v>2.50918</v>
+        <v>2.83227</v>
       </c>
       <c r="AG8">
-        <v>2.6978</v>
+        <v>3.0326</v>
       </c>
       <c r="AK8" t="s">
         <v>8</v>
       </c>
       <c r="AL8">
-        <v>2.90064</v>
+        <v>2.73851</v>
       </c>
       <c r="AM8">
-        <v>3.0814</v>
+        <v>2.9194</v>
       </c>
       <c r="AQ8" t="s">
         <v>8</v>
       </c>
       <c r="AR8">
-        <v>3.4898</v>
+        <v>3.46338</v>
       </c>
       <c r="AS8">
-        <v>3.6426</v>
+        <v>3.6399</v>
       </c>
       <c r="AW8" t="s">
         <v>8</v>
       </c>
       <c r="AX8">
-        <v>4.48944</v>
+        <v>4.49116</v>
       </c>
       <c r="AY8">
-        <v>4.6507</v>
+        <v>4.647</v>
       </c>
       <c r="BC8" t="s">
         <v>8</v>
       </c>
       <c r="BD8">
-        <v>7.81361</v>
+        <v>4.37049</v>
       </c>
       <c r="BE8">
-        <v>7.9142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:57">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
+        <v>4.5248</v>
+      </c>
+    </row>
+    <row r="9" spans="7:57">
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9">
-        <v>0.41772</v>
+        <v>0.35685</v>
       </c>
       <c r="I9">
-        <v>0.6555</v>
+        <v>0.6115</v>
       </c>
       <c r="M9" t="s">
         <v>9</v>
       </c>
       <c r="N9">
-        <v>0.88545</v>
+        <v>0.54637</v>
       </c>
       <c r="O9">
-        <v>1.1081</v>
+        <v>0.7772</v>
       </c>
       <c r="S9" t="s">
         <v>9</v>
       </c>
       <c r="T9">
-        <v>1.18272</v>
+        <v>1.09418</v>
       </c>
       <c r="U9">
-        <v>1.3868</v>
+        <v>1.3119</v>
       </c>
       <c r="Y9" t="s">
         <v>9</v>
       </c>
       <c r="Z9">
-        <v>2.1542</v>
+        <v>2.25454</v>
       </c>
       <c r="AA9">
-        <v>2.3569</v>
+        <v>2.493</v>
       </c>
       <c r="AE9" t="s">
         <v>9</v>
       </c>
       <c r="AF9">
-        <v>2.12587</v>
+        <v>2.51426</v>
       </c>
       <c r="AG9">
-        <v>2.3181</v>
+        <v>2.7043</v>
       </c>
       <c r="AK9" t="s">
         <v>9</v>
       </c>
       <c r="AL9">
-        <v>2.98749</v>
+        <v>2.72037</v>
       </c>
       <c r="AM9">
-        <v>3.1577</v>
+        <v>2.9153</v>
       </c>
       <c r="AQ9" t="s">
         <v>9</v>
       </c>
       <c r="AR9">
-        <v>3.38471</v>
+        <v>3.22282</v>
       </c>
       <c r="AS9">
-        <v>3.5378</v>
+        <v>3.3888</v>
       </c>
       <c r="AW9" t="s">
         <v>9</v>
       </c>
       <c r="AX9">
-        <v>4.23556</v>
+        <v>4.02959</v>
       </c>
       <c r="AY9">
-        <v>4.3871</v>
+        <v>4.1936</v>
       </c>
       <c r="BC9" t="s">
         <v>9</v>
       </c>
       <c r="BD9">
-        <v>6.95303</v>
+        <v>4.5477</v>
       </c>
       <c r="BE9">
-        <v>6.8617</v>
-      </c>
-    </row>
-    <row r="10" spans="1:57">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
+        <v>4.6983</v>
+      </c>
+    </row>
+    <row r="10" spans="7:57">
       <c r="G10" t="s">
         <v>10</v>
       </c>
       <c r="H10">
-        <v>0.4398</v>
+        <v>0.31857</v>
       </c>
       <c r="I10">
-        <v>0.6765</v>
+        <v>0.5731000000000001</v>
       </c>
       <c r="M10" t="s">
         <v>10</v>
       </c>
       <c r="N10">
-        <v>0.88423</v>
+        <v>1.28719</v>
       </c>
       <c r="O10">
-        <v>1.1085</v>
+        <v>1.5148</v>
       </c>
       <c r="S10" t="s">
         <v>10</v>
       </c>
       <c r="T10">
-        <v>1.07139</v>
+        <v>1.03162</v>
       </c>
       <c r="U10">
-        <v>1.2808</v>
+        <v>1.2518</v>
       </c>
       <c r="Y10" t="s">
         <v>10</v>
       </c>
       <c r="Z10">
-        <v>2.07682</v>
+        <v>1.71655</v>
       </c>
       <c r="AA10">
-        <v>2.2779</v>
+        <v>1.9448</v>
       </c>
       <c r="AE10" t="s">
         <v>10</v>
       </c>
       <c r="AF10">
-        <v>2.81567</v>
+        <v>2.80774</v>
       </c>
       <c r="AG10">
-        <v>3.0034</v>
+        <v>3.0477</v>
       </c>
       <c r="AK10" t="s">
         <v>10</v>
       </c>
       <c r="AL10">
-        <v>3.06544</v>
+        <v>2.72609</v>
       </c>
       <c r="AM10">
-        <v>3.2459</v>
+        <v>2.9138</v>
       </c>
       <c r="AQ10" t="s">
         <v>10</v>
       </c>
       <c r="AR10">
-        <v>3.68096</v>
+        <v>3.2523</v>
       </c>
       <c r="AS10">
-        <v>3.8331</v>
+        <v>3.428</v>
       </c>
       <c r="AW10" t="s">
         <v>10</v>
       </c>
       <c r="AX10">
-        <v>4.24782</v>
+        <v>4.19231</v>
       </c>
       <c r="AY10">
-        <v>4.4767</v>
+        <v>4.3377</v>
       </c>
       <c r="BC10" t="s">
         <v>10</v>
       </c>
       <c r="BD10">
-        <v>7.24949</v>
+        <v>7.30318</v>
       </c>
       <c r="BE10">
-        <v>7.3683</v>
-      </c>
-    </row>
-    <row r="11" spans="1:57">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
+        <v>7.443</v>
+      </c>
+    </row>
+    <row r="11" spans="7:57">
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11">
-        <v>0.65527</v>
+        <v>0.30202</v>
       </c>
       <c r="I11">
-        <v>0.8917</v>
+        <v>0.5563</v>
       </c>
       <c r="M11" t="s">
         <v>11</v>
       </c>
       <c r="N11">
-        <v>0.74408</v>
+        <v>0.59497</v>
       </c>
       <c r="O11">
-        <v>0.9666</v>
+        <v>0.8214</v>
       </c>
       <c r="S11" t="s">
         <v>11</v>
       </c>
       <c r="T11">
-        <v>2.04616</v>
+        <v>0.83396</v>
       </c>
       <c r="U11">
-        <v>2.252</v>
+        <v>1.0581</v>
       </c>
       <c r="Y11" t="s">
         <v>11</v>
       </c>
       <c r="Z11">
-        <v>2.13377</v>
+        <v>2.05687</v>
       </c>
       <c r="AA11">
-        <v>2.3322</v>
+        <v>2.2578</v>
       </c>
       <c r="AE11" t="s">
         <v>11</v>
       </c>
       <c r="AF11">
-        <v>2.49756</v>
+        <v>2.43811</v>
       </c>
       <c r="AG11">
-        <v>2.6797</v>
+        <v>2.6366</v>
       </c>
       <c r="AK11" t="s">
         <v>11</v>
       </c>
       <c r="AL11">
-        <v>2.77749</v>
+        <v>2.86011</v>
       </c>
       <c r="AM11">
-        <v>2.9468</v>
+        <v>3.0499</v>
       </c>
       <c r="AQ11" t="s">
         <v>11</v>
       </c>
       <c r="AR11">
-        <v>3.45263</v>
+        <v>3.2794</v>
       </c>
       <c r="AS11">
-        <v>3.5972</v>
+        <v>3.4489</v>
       </c>
       <c r="AW11" t="s">
         <v>11</v>
       </c>
       <c r="AX11">
-        <v>4.17861</v>
+        <v>4.09959</v>
       </c>
       <c r="AY11">
-        <v>4.4052</v>
+        <v>4.2503</v>
       </c>
       <c r="BC11" t="s">
         <v>11</v>
       </c>
       <c r="BD11">
-        <v>6.37218</v>
+        <v>4.10435</v>
       </c>
       <c r="BE11">
-        <v>6.5117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:57">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
+        <v>4.2615</v>
+      </c>
+    </row>
+    <row r="12" spans="7:57">
       <c r="G12" t="s">
         <v>12</v>
       </c>
       <c r="H12">
-        <v>0.42522</v>
+        <v>0.36779</v>
       </c>
       <c r="I12">
-        <v>0.6605</v>
+        <v>0.6224</v>
       </c>
       <c r="M12" t="s">
         <v>12</v>
       </c>
       <c r="N12">
-        <v>0.79172</v>
+        <v>0.59758</v>
       </c>
       <c r="O12">
-        <v>1.0162</v>
+        <v>0.8277</v>
       </c>
       <c r="S12" t="s">
         <v>12</v>
       </c>
       <c r="T12">
-        <v>1.05752</v>
+        <v>0.86777</v>
       </c>
       <c r="U12">
-        <v>1.2655</v>
+        <v>1.0906</v>
       </c>
       <c r="Y12" t="s">
         <v>12</v>
       </c>
       <c r="Z12">
-        <v>2.13728</v>
+        <v>1.7557</v>
       </c>
       <c r="AA12">
-        <v>2.3423</v>
+        <v>1.9657</v>
       </c>
       <c r="AE12" t="s">
         <v>12</v>
       </c>
       <c r="AF12">
-        <v>2.34323</v>
+        <v>2.33883</v>
       </c>
       <c r="AG12">
-        <v>2.5306</v>
+        <v>2.5383</v>
       </c>
       <c r="AK12" t="s">
         <v>12</v>
       </c>
       <c r="AL12">
-        <v>2.63833</v>
+        <v>4.16223</v>
       </c>
       <c r="AM12">
-        <v>2.8131</v>
+        <v>4.3573</v>
       </c>
       <c r="AQ12" t="s">
         <v>12</v>
       </c>
       <c r="AR12">
-        <v>3.16922</v>
+        <v>3.24553</v>
       </c>
       <c r="AS12">
-        <v>3.3083</v>
+        <v>3.415</v>
       </c>
       <c r="AW12" t="s">
         <v>12</v>
       </c>
       <c r="AX12">
-        <v>4.24247</v>
+        <v>4.55115</v>
       </c>
       <c r="AY12">
-        <v>4.3947</v>
+        <v>4.7198</v>
       </c>
       <c r="BC12" t="s">
         <v>12</v>
       </c>
       <c r="BD12">
-        <v>6.62029</v>
+        <v>6.57092</v>
       </c>
       <c r="BE12">
-        <v>6.7098</v>
-      </c>
-    </row>
-    <row r="13" spans="1:57">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
+        <v>6.7325</v>
+      </c>
+    </row>
+    <row r="13" spans="7:57">
       <c r="G13" t="s">
         <v>13</v>
       </c>
       <c r="H13">
-        <v>0.47633</v>
+        <v>0.48279</v>
       </c>
       <c r="I13">
-        <v>0.7095</v>
+        <v>0.7374000000000001</v>
       </c>
       <c r="M13" t="s">
         <v>13</v>
       </c>
       <c r="N13">
-        <v>0.7098</v>
+        <v>0.54203</v>
       </c>
       <c r="O13">
-        <v>0.9352</v>
+        <v>0.7724</v>
       </c>
       <c r="S13" t="s">
         <v>13</v>
       </c>
       <c r="T13">
-        <v>1.33199</v>
+        <v>0.86553</v>
       </c>
       <c r="U13">
-        <v>1.5397</v>
+        <v>1.0874</v>
       </c>
       <c r="Y13" t="s">
         <v>13</v>
       </c>
       <c r="Z13">
-        <v>1.595</v>
+        <v>1.95416</v>
       </c>
       <c r="AA13">
-        <v>1.7956</v>
+        <v>2.1988</v>
       </c>
       <c r="AE13" t="s">
         <v>13</v>
       </c>
       <c r="AF13">
-        <v>2.318</v>
+        <v>2.53169</v>
       </c>
       <c r="AG13">
-        <v>2.4955</v>
+        <v>2.7274</v>
       </c>
       <c r="AK13" t="s">
         <v>13</v>
       </c>
       <c r="AL13">
-        <v>3.08113</v>
+        <v>2.68651</v>
       </c>
       <c r="AM13">
-        <v>3.2502</v>
+        <v>2.8762</v>
       </c>
       <c r="AQ13" t="s">
         <v>13</v>
       </c>
       <c r="AR13">
-        <v>3.62408</v>
+        <v>3.29379</v>
       </c>
       <c r="AS13">
-        <v>3.7749</v>
+        <v>3.4315</v>
       </c>
       <c r="AW13" t="s">
         <v>13</v>
       </c>
       <c r="AX13">
-        <v>4.11894</v>
+        <v>4.48127</v>
       </c>
       <c r="AY13">
-        <v>4.2588</v>
+        <v>4.6554</v>
       </c>
       <c r="BC13" t="s">
         <v>13</v>
       </c>
       <c r="BD13">
-        <v>5.53953</v>
+        <v>4.39367</v>
       </c>
       <c r="BE13">
-        <v>5.7048</v>
-      </c>
-    </row>
-    <row r="14" spans="1:57">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
+        <v>4.6172</v>
+      </c>
+    </row>
+    <row r="14" spans="7:57">
       <c r="G14" t="s">
         <v>14</v>
       </c>
       <c r="H14">
-        <v>0.45216</v>
+        <v>0.4561</v>
       </c>
       <c r="I14">
-        <v>0.6853</v>
+        <v>0.7096</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
       </c>
       <c r="N14">
-        <v>0.79844</v>
+        <v>0.66315</v>
       </c>
       <c r="O14">
-        <v>1.0245</v>
+        <v>0.8931</v>
       </c>
       <c r="S14" t="s">
         <v>14</v>
       </c>
       <c r="T14">
-        <v>1.26602</v>
+        <v>0.9227</v>
       </c>
       <c r="U14">
-        <v>1.4739</v>
+        <v>1.1446</v>
       </c>
       <c r="Y14" t="s">
         <v>14</v>
       </c>
       <c r="Z14">
-        <v>2.19032</v>
+        <v>2.06386</v>
       </c>
       <c r="AA14">
-        <v>2.3932</v>
+        <v>2.2638</v>
       </c>
       <c r="AE14" t="s">
         <v>14</v>
       </c>
       <c r="AF14">
-        <v>2.46578</v>
+        <v>2.40497</v>
       </c>
       <c r="AG14">
-        <v>2.6493</v>
+        <v>2.6027</v>
       </c>
       <c r="AK14" t="s">
         <v>14</v>
       </c>
       <c r="AL14">
-        <v>2.93228</v>
+        <v>2.84598</v>
       </c>
       <c r="AM14">
-        <v>3.1028</v>
+        <v>3.0351</v>
       </c>
       <c r="AQ14" t="s">
         <v>14</v>
       </c>
       <c r="AR14">
-        <v>3.1631</v>
+        <v>3.84975</v>
       </c>
       <c r="AS14">
-        <v>3.3194</v>
+        <v>4.0658</v>
       </c>
       <c r="AW14" t="s">
         <v>14</v>
       </c>
       <c r="AX14">
-        <v>3.95925</v>
+        <v>4.28793</v>
       </c>
       <c r="AY14">
-        <v>4.1065</v>
+        <v>4.4534</v>
       </c>
       <c r="BC14" t="s">
         <v>14</v>
       </c>
       <c r="BD14">
-        <v>6.68247</v>
+        <v>4.26738</v>
       </c>
       <c r="BE14">
-        <v>6.7699</v>
-      </c>
-    </row>
-    <row r="15" spans="1:57">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
+        <v>4.4249</v>
+      </c>
+    </row>
+    <row r="15" spans="7:57">
       <c r="G15" t="s">
         <v>15</v>
       </c>
       <c r="H15">
-        <v>0.46187</v>
+        <v>0.35708</v>
       </c>
       <c r="I15">
-        <v>0.6952</v>
+        <v>0.6</v>
       </c>
       <c r="M15" t="s">
         <v>15</v>
       </c>
       <c r="N15">
-        <v>0.7831</v>
+        <v>0.9926</v>
       </c>
       <c r="O15">
-        <v>1.0083</v>
+        <v>1.2238</v>
       </c>
       <c r="S15" t="s">
         <v>15</v>
       </c>
       <c r="T15">
-        <v>1.28554</v>
+        <v>1.90059</v>
       </c>
       <c r="U15">
-        <v>1.4968</v>
+        <v>2.1239</v>
       </c>
       <c r="Y15" t="s">
         <v>15</v>
       </c>
       <c r="Z15">
-        <v>2.15081</v>
+        <v>1.96129</v>
       </c>
       <c r="AA15">
-        <v>2.3929</v>
+        <v>2.2029</v>
       </c>
       <c r="AE15" t="s">
         <v>15</v>
       </c>
       <c r="AF15">
-        <v>2.48199</v>
+        <v>2.42648</v>
       </c>
       <c r="AG15">
-        <v>2.6712</v>
+        <v>2.6264</v>
       </c>
       <c r="AK15" t="s">
         <v>15</v>
       </c>
       <c r="AL15">
-        <v>2.74469</v>
+        <v>2.71702</v>
       </c>
       <c r="AM15">
-        <v>2.9192</v>
+        <v>2.9091</v>
       </c>
       <c r="AQ15" t="s">
         <v>15</v>
       </c>
       <c r="AR15">
-        <v>3.38568</v>
+        <v>3.33281</v>
       </c>
       <c r="AS15">
-        <v>3.5357</v>
+        <v>3.5034</v>
       </c>
       <c r="AW15" t="s">
         <v>15</v>
       </c>
       <c r="AX15">
-        <v>3.98102</v>
+        <v>3.95613</v>
       </c>
       <c r="AY15">
-        <v>4.1254</v>
+        <v>4.1192</v>
       </c>
       <c r="BC15" t="s">
         <v>15</v>
       </c>
       <c r="BD15">
-        <v>5.43718</v>
+        <v>4.29136</v>
       </c>
       <c r="BE15">
-        <v>5.5427</v>
-      </c>
-    </row>
-    <row r="16" spans="1:57">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
+        <v>4.436</v>
+      </c>
+    </row>
+    <row r="16" spans="7:57">
       <c r="G16" t="s">
         <v>16</v>
       </c>
       <c r="H16">
-        <v>0.44001</v>
+        <v>0.345</v>
       </c>
       <c r="I16">
-        <v>0.6758</v>
+        <v>0.5866</v>
       </c>
       <c r="M16" t="s">
         <v>16</v>
       </c>
       <c r="N16">
-        <v>0.68003</v>
+        <v>1.0764</v>
       </c>
       <c r="O16">
-        <v>0.9051</v>
+        <v>1.3024</v>
       </c>
       <c r="S16" t="s">
         <v>16</v>
       </c>
       <c r="T16">
-        <v>1.64471</v>
+        <v>1.47892</v>
       </c>
       <c r="U16">
-        <v>1.8903</v>
+        <v>1.6957</v>
       </c>
       <c r="Y16" t="s">
         <v>16</v>
       </c>
       <c r="Z16">
-        <v>1.95012</v>
+        <v>1.78498</v>
       </c>
       <c r="AA16">
-        <v>2.1934</v>
+        <v>2.028</v>
       </c>
       <c r="AE16" t="s">
         <v>16</v>
       </c>
       <c r="AF16">
-        <v>2.26583</v>
+        <v>3.92486</v>
       </c>
       <c r="AG16">
-        <v>2.4498</v>
+        <v>4.122</v>
       </c>
       <c r="AK16" t="s">
         <v>16</v>
       </c>
       <c r="AL16">
-        <v>2.81347</v>
+        <v>2.51479</v>
       </c>
       <c r="AM16">
-        <v>2.9861</v>
+        <v>2.6969</v>
       </c>
       <c r="AQ16" t="s">
         <v>16</v>
       </c>
       <c r="AR16">
-        <v>3.47305</v>
+        <v>3.66179</v>
       </c>
       <c r="AS16">
-        <v>3.6254</v>
+        <v>3.8391</v>
       </c>
       <c r="AW16" t="s">
         <v>16</v>
       </c>
       <c r="AX16">
-        <v>3.79414</v>
+        <v>4.47675</v>
       </c>
       <c r="AY16">
-        <v>3.9481</v>
+        <v>4.6436</v>
       </c>
       <c r="BC16" t="s">
         <v>16</v>
       </c>
       <c r="BD16">
-        <v>4.73682</v>
+        <v>4.37854</v>
       </c>
       <c r="BE16">
-        <v>4.9679</v>
-      </c>
-    </row>
-    <row r="17" spans="1:57">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
+        <v>4.5385</v>
+      </c>
+    </row>
+    <row r="17" spans="7:57">
       <c r="G17" t="s">
         <v>17</v>
       </c>
       <c r="H17">
-        <v>0.46752</v>
+        <v>0.33649</v>
       </c>
       <c r="I17">
-        <v>0.7006</v>
+        <v>0.5784</v>
       </c>
       <c r="M17" t="s">
         <v>17</v>
       </c>
       <c r="N17">
-        <v>0.66234</v>
+        <v>0.69753</v>
       </c>
       <c r="O17">
-        <v>0.8915999999999999</v>
+        <v>0.927</v>
       </c>
       <c r="S17" t="s">
         <v>17</v>
       </c>
       <c r="T17">
-        <v>1.13309</v>
+        <v>1.06817</v>
       </c>
       <c r="U17">
-        <v>1.3044</v>
+        <v>1.2856</v>
       </c>
       <c r="Y17" t="s">
         <v>17</v>
       </c>
       <c r="Z17">
-        <v>1.57375</v>
+        <v>1.75274</v>
       </c>
       <c r="AA17">
-        <v>1.8157</v>
+        <v>1.9594</v>
       </c>
       <c r="AE17" t="s">
         <v>17</v>
       </c>
       <c r="AF17">
-        <v>2.52033</v>
+        <v>2.47086</v>
       </c>
       <c r="AG17">
-        <v>2.7019</v>
+        <v>2.6676</v>
       </c>
       <c r="AK17" t="s">
         <v>17</v>
       </c>
       <c r="AL17">
-        <v>4.53512</v>
+        <v>2.88907</v>
       </c>
       <c r="AM17">
-        <v>4.712</v>
+        <v>3.0693</v>
       </c>
       <c r="AQ17" t="s">
         <v>17</v>
       </c>
       <c r="AR17">
-        <v>3.33945</v>
+        <v>3.30556</v>
       </c>
       <c r="AS17">
-        <v>3.4868</v>
+        <v>3.4755</v>
       </c>
       <c r="AW17" t="s">
         <v>17</v>
       </c>
       <c r="AX17">
-        <v>3.67818</v>
+        <v>5.98645</v>
       </c>
       <c r="AY17">
-        <v>3.8238</v>
+        <v>6.1487</v>
       </c>
       <c r="BC17" t="s">
         <v>17</v>
       </c>
       <c r="BD17">
-        <v>4.69562</v>
+        <v>4.56846</v>
       </c>
       <c r="BE17">
-        <v>4.8687</v>
-      </c>
-    </row>
-    <row r="18" spans="1:57">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
+        <v>4.7223</v>
+      </c>
+    </row>
+    <row r="18" spans="7:57">
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18">
-        <v>0.94056</v>
+        <v>0.33086</v>
       </c>
       <c r="I18">
-        <v>1.1765</v>
+        <v>0.5725</v>
       </c>
       <c r="M18" t="s">
         <v>18</v>
       </c>
       <c r="N18">
-        <v>0.57723</v>
+        <v>0.59628</v>
       </c>
       <c r="O18">
-        <v>0.8063</v>
+        <v>0.827</v>
       </c>
       <c r="S18" t="s">
         <v>18</v>
       </c>
       <c r="T18">
-        <v>1.16597</v>
+        <v>0.93518</v>
       </c>
       <c r="U18">
-        <v>1.3756</v>
+        <v>1.1558</v>
       </c>
       <c r="Y18" t="s">
         <v>18</v>
       </c>
       <c r="Z18">
-        <v>2.03631</v>
+        <v>2.31155</v>
       </c>
       <c r="AA18">
-        <v>2.2799</v>
+        <v>2.511</v>
       </c>
       <c r="AE18" t="s">
         <v>18</v>
       </c>
       <c r="AF18">
-        <v>2.52553</v>
+        <v>2.64383</v>
       </c>
       <c r="AG18">
-        <v>2.7075</v>
+        <v>2.8395</v>
       </c>
       <c r="AK18" t="s">
         <v>18</v>
       </c>
       <c r="AL18">
-        <v>3.08823</v>
+        <v>4.60063</v>
       </c>
       <c r="AM18">
-        <v>3.2601</v>
+        <v>4.7856</v>
       </c>
       <c r="AQ18" t="s">
         <v>18</v>
       </c>
       <c r="AR18">
-        <v>3.26705</v>
+        <v>3.39307</v>
       </c>
       <c r="AS18">
-        <v>3.4511</v>
+        <v>3.598</v>
       </c>
       <c r="AW18" t="s">
         <v>18</v>
       </c>
       <c r="AX18">
-        <v>3.91601</v>
+        <v>4.53563</v>
       </c>
       <c r="AY18">
-        <v>4.0652</v>
+        <v>4.7523</v>
       </c>
       <c r="BC18" t="s">
         <v>18</v>
       </c>
       <c r="BD18">
-        <v>4.64063</v>
+        <v>4.21808</v>
       </c>
       <c r="BE18">
-        <v>4.7817</v>
-      </c>
-    </row>
-    <row r="19" spans="1:57">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
+        <v>4.3563</v>
+      </c>
+    </row>
+    <row r="19" spans="7:57">
       <c r="G19" t="s">
         <v>19</v>
       </c>
       <c r="H19">
-        <v>0.56426</v>
+        <v>0.34593</v>
       </c>
       <c r="I19">
-        <v>0.7976</v>
+        <v>0.5872000000000001</v>
       </c>
       <c r="M19" t="s">
         <v>19</v>
       </c>
       <c r="N19">
-        <v>0.68546</v>
+        <v>0.59466</v>
       </c>
       <c r="O19">
-        <v>0.9129</v>
+        <v>0.8253</v>
       </c>
       <c r="S19" t="s">
         <v>19</v>
       </c>
       <c r="T19">
-        <v>1.39491</v>
+        <v>1.00726</v>
       </c>
       <c r="U19">
-        <v>1.6058</v>
+        <v>1.228</v>
       </c>
       <c r="Y19" t="s">
         <v>19</v>
       </c>
       <c r="Z19">
-        <v>1.9396</v>
+        <v>2.02038</v>
       </c>
       <c r="AA19">
-        <v>2.1794</v>
+        <v>2.2286</v>
       </c>
       <c r="AE19" t="s">
         <v>19</v>
       </c>
       <c r="AF19">
-        <v>2.36343</v>
+        <v>2.69754</v>
       </c>
       <c r="AG19">
-        <v>2.5479</v>
+        <v>2.8998</v>
       </c>
       <c r="AK19" t="s">
         <v>19</v>
       </c>
       <c r="AL19">
-        <v>4.52677</v>
+        <v>2.8961</v>
       </c>
       <c r="AM19">
-        <v>4.7032</v>
+        <v>3.0788</v>
       </c>
       <c r="AQ19" t="s">
         <v>19</v>
       </c>
       <c r="AR19">
-        <v>3.03575</v>
+        <v>3.81336</v>
       </c>
       <c r="AS19">
-        <v>3.1972</v>
+        <v>4.0016</v>
       </c>
       <c r="AW19" t="s">
         <v>19</v>
       </c>
       <c r="AX19">
-        <v>3.77309</v>
+        <v>4.44648</v>
       </c>
       <c r="AY19">
-        <v>3.9106</v>
+        <v>4.6144</v>
       </c>
       <c r="BC19" t="s">
         <v>19</v>
       </c>
       <c r="BD19">
-        <v>5.1946</v>
+        <v>4.24008</v>
       </c>
       <c r="BE19">
-        <v>5.3174</v>
-      </c>
-    </row>
-    <row r="20" spans="1:57">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
+        <v>4.3963</v>
+      </c>
+    </row>
+    <row r="20" spans="7:57">
       <c r="G20" t="s">
         <v>20</v>
       </c>
       <c r="H20">
-        <v>0.50238</v>
+        <v>0.37259</v>
       </c>
       <c r="I20">
-        <v>0.7349</v>
+        <v>0.6143</v>
       </c>
       <c r="M20" t="s">
         <v>20</v>
       </c>
       <c r="N20">
-        <v>0.7692600000000001</v>
+        <v>0.55606</v>
       </c>
       <c r="O20">
-        <v>0.9933999999999999</v>
+        <v>0.7842</v>
       </c>
       <c r="S20" t="s">
         <v>20</v>
       </c>
       <c r="T20">
-        <v>1.20015</v>
+        <v>0.87265</v>
       </c>
       <c r="U20">
-        <v>1.4102</v>
+        <v>1.0963</v>
       </c>
       <c r="Y20" t="s">
         <v>20</v>
       </c>
       <c r="Z20">
-        <v>2.25016</v>
+        <v>2.03219</v>
       </c>
       <c r="AA20">
-        <v>2.4463</v>
+        <v>2.2342</v>
       </c>
       <c r="AE20" t="s">
         <v>20</v>
       </c>
       <c r="AF20">
-        <v>2.42213</v>
+        <v>2.59859</v>
       </c>
       <c r="AG20">
-        <v>2.6118</v>
+        <v>2.7926</v>
       </c>
       <c r="AK20" t="s">
         <v>20</v>
       </c>
       <c r="AL20">
-        <v>2.91482</v>
+        <v>2.72536</v>
       </c>
       <c r="AM20">
-        <v>3.0795</v>
+        <v>2.9095</v>
       </c>
       <c r="AQ20" t="s">
         <v>20</v>
       </c>
       <c r="AR20">
-        <v>3.10081</v>
+        <v>3.1053</v>
       </c>
       <c r="AS20">
-        <v>3.2793</v>
+        <v>3.3355</v>
       </c>
       <c r="AW20" t="s">
         <v>20</v>
       </c>
       <c r="AX20">
-        <v>3.78545</v>
+        <v>4.17704</v>
       </c>
       <c r="AY20">
-        <v>3.9276</v>
+        <v>4.3455</v>
       </c>
       <c r="BC20" t="s">
         <v>20</v>
       </c>
       <c r="BD20">
-        <v>4.79104</v>
+        <v>4.58716</v>
       </c>
       <c r="BE20">
-        <v>4.9057</v>
-      </c>
-    </row>
-    <row r="21" spans="1:57">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
+        <v>4.7273</v>
+      </c>
+    </row>
+    <row r="21" spans="7:57">
       <c r="G21" t="s">
         <v>21</v>
       </c>
       <c r="H21">
-        <v>0.59933</v>
+        <v>0.40634</v>
       </c>
       <c r="I21">
-        <v>0.8371</v>
+        <v>0.6487000000000001</v>
       </c>
       <c r="M21" t="s">
         <v>21</v>
       </c>
       <c r="N21">
-        <v>0.86015</v>
+        <v>0.58802</v>
       </c>
       <c r="O21">
-        <v>1.0836</v>
+        <v>0.8186</v>
       </c>
       <c r="S21" t="s">
         <v>21</v>
       </c>
       <c r="T21">
-        <v>1.28363</v>
+        <v>1.28326</v>
       </c>
       <c r="U21">
-        <v>1.4933</v>
+        <v>1.5024</v>
       </c>
       <c r="Y21" t="s">
         <v>21</v>
       </c>
       <c r="Z21">
-        <v>2.02796</v>
+        <v>2.06176</v>
       </c>
       <c r="AA21">
-        <v>2.223</v>
+        <v>2.2661</v>
       </c>
       <c r="AE21" t="s">
         <v>21</v>
       </c>
       <c r="AF21">
-        <v>2.21094</v>
+        <v>3.79437</v>
       </c>
       <c r="AG21">
-        <v>2.4025</v>
+        <v>4.031</v>
       </c>
       <c r="AK21" t="s">
         <v>21</v>
       </c>
       <c r="AL21">
-        <v>3.62007</v>
+        <v>2.7446</v>
       </c>
       <c r="AM21">
-        <v>3.7914</v>
+        <v>2.9311</v>
       </c>
       <c r="AQ21" t="s">
         <v>21</v>
       </c>
       <c r="AR21">
-        <v>3.14944</v>
+        <v>3.33922</v>
       </c>
       <c r="AS21">
-        <v>3.3184</v>
+        <v>3.5682</v>
       </c>
       <c r="AW21" t="s">
         <v>21</v>
       </c>
       <c r="AX21">
-        <v>3.94833</v>
+        <v>4.3283</v>
       </c>
       <c r="AY21">
-        <v>4.0794</v>
+        <v>4.4786</v>
       </c>
       <c r="BC21" t="s">
         <v>21</v>
       </c>
       <c r="BD21">
-        <v>5.36607</v>
+        <v>4.3366</v>
       </c>
       <c r="BE21">
-        <v>5.4933</v>
-      </c>
-    </row>
-    <row r="22" spans="1:57">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
+        <v>4.4951</v>
+      </c>
+    </row>
+    <row r="22" spans="7:57">
       <c r="G22" t="s">
         <v>22</v>
       </c>
       <c r="H22">
-        <v>0.48534</v>
+        <v>0.32637</v>
       </c>
       <c r="I22">
-        <v>0.7136</v>
+        <v>0.5676</v>
       </c>
       <c r="M22" t="s">
         <v>22</v>
       </c>
       <c r="N22">
-        <v>0.75681</v>
+        <v>0.80953</v>
       </c>
       <c r="O22">
-        <v>0.9831</v>
+        <v>1.0393</v>
       </c>
       <c r="S22" t="s">
         <v>22</v>
       </c>
       <c r="T22">
-        <v>1.27574</v>
+        <v>0.87275</v>
       </c>
       <c r="U22">
-        <v>1.4892</v>
+        <v>1.0956</v>
       </c>
       <c r="Y22" t="s">
         <v>22</v>
       </c>
       <c r="Z22">
-        <v>1.70609</v>
+        <v>1.96536</v>
       </c>
       <c r="AA22">
-        <v>1.9489</v>
+        <v>2.1656</v>
       </c>
       <c r="AE22" t="s">
         <v>22</v>
       </c>
       <c r="AF22">
-        <v>2.22342</v>
+        <v>2.42115</v>
       </c>
       <c r="AG22">
-        <v>2.416</v>
+        <v>2.62</v>
       </c>
       <c r="AK22" t="s">
         <v>22</v>
       </c>
       <c r="AL22">
-        <v>2.97047</v>
+        <v>2.97293</v>
       </c>
       <c r="AM22">
-        <v>3.0462</v>
+        <v>3.1513</v>
       </c>
       <c r="AQ22" t="s">
         <v>22</v>
       </c>
       <c r="AR22">
-        <v>3.60791</v>
+        <v>3.35237</v>
       </c>
       <c r="AS22">
-        <v>3.7661</v>
+        <v>3.5873</v>
       </c>
       <c r="AW22" t="s">
         <v>22</v>
       </c>
       <c r="AX22">
-        <v>4.4943</v>
+        <v>3.87633</v>
       </c>
       <c r="AY22">
-        <v>4.623</v>
+        <v>4.1044</v>
       </c>
       <c r="BC22" t="s">
         <v>22</v>
       </c>
       <c r="BD22">
-        <v>4.44382</v>
+        <v>4.21526</v>
       </c>
       <c r="BE22">
-        <v>4.6669</v>
-      </c>
-    </row>
-    <row r="23" spans="1:57">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
+        <v>4.36</v>
+      </c>
+    </row>
+    <row r="23" spans="7:57">
       <c r="G23" t="s">
         <v>23</v>
       </c>
       <c r="H23">
-        <v>0.73674</v>
+        <v>0.32974</v>
       </c>
       <c r="I23">
-        <v>0.9744</v>
+        <v>0.5721000000000001</v>
       </c>
       <c r="M23" t="s">
         <v>23</v>
       </c>
       <c r="N23">
-        <v>1.0028</v>
+        <v>0.7676500000000001</v>
       </c>
       <c r="O23">
-        <v>1.221</v>
+        <v>0.9957</v>
       </c>
       <c r="S23" t="s">
         <v>23</v>
       </c>
       <c r="T23">
-        <v>1.32173</v>
+        <v>1.06373</v>
       </c>
       <c r="U23">
-        <v>1.5326</v>
+        <v>1.2821</v>
       </c>
       <c r="Y23" t="s">
         <v>23</v>
       </c>
       <c r="Z23">
-        <v>1.95302</v>
+        <v>1.9835</v>
       </c>
       <c r="AA23">
-        <v>2.1485</v>
+        <v>2.1913</v>
       </c>
       <c r="AE23" t="s">
         <v>23</v>
       </c>
       <c r="AF23">
-        <v>2.29673</v>
+        <v>2.56271</v>
       </c>
       <c r="AG23">
-        <v>2.4771</v>
+        <v>2.7572</v>
       </c>
       <c r="AK23" t="s">
         <v>23</v>
       </c>
       <c r="AL23">
-        <v>2.86728</v>
+        <v>2.82867</v>
       </c>
       <c r="AM23">
-        <v>3.0806</v>
+        <v>3.0202</v>
       </c>
       <c r="AQ23" t="s">
         <v>23</v>
       </c>
       <c r="AR23">
-        <v>3.23411</v>
+        <v>3.13809</v>
       </c>
       <c r="AS23">
-        <v>3.4656</v>
+        <v>3.3708</v>
       </c>
       <c r="AW23" t="s">
         <v>23</v>
       </c>
       <c r="AX23">
-        <v>3.97965</v>
+        <v>4.81322</v>
       </c>
       <c r="AY23">
-        <v>4.091</v>
+        <v>4.9959</v>
       </c>
       <c r="BC23" t="s">
         <v>23</v>
       </c>
       <c r="BD23">
-        <v>4.58005</v>
+        <v>4.18838</v>
       </c>
       <c r="BE23">
-        <v>4.7126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:57">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
+        <v>4.3446</v>
+      </c>
+    </row>
+    <row r="24" spans="7:57">
       <c r="G24" t="s">
         <v>24</v>
       </c>
       <c r="H24">
-        <v>0.70868</v>
+        <v>0.33826</v>
       </c>
       <c r="I24">
-        <v>0.9471000000000001</v>
+        <v>0.5803</v>
       </c>
       <c r="M24" t="s">
         <v>24</v>
       </c>
       <c r="N24">
-        <v>0.72473</v>
+        <v>0.64621</v>
       </c>
       <c r="O24">
-        <v>0.9451000000000001</v>
+        <v>0.8754</v>
       </c>
       <c r="S24" t="s">
         <v>24</v>
       </c>
       <c r="T24">
-        <v>1.34035</v>
+        <v>1.31931</v>
       </c>
       <c r="U24">
-        <v>1.5529</v>
+        <v>1.543</v>
       </c>
       <c r="Y24" t="s">
         <v>24</v>
       </c>
       <c r="Z24">
-        <v>1.66385</v>
+        <v>1.43446</v>
       </c>
       <c r="AA24">
-        <v>1.8345</v>
+        <v>1.6445</v>
       </c>
       <c r="AE24" t="s">
         <v>24</v>
       </c>
       <c r="AF24">
-        <v>2.46178</v>
+        <v>2.56469</v>
       </c>
       <c r="AG24">
-        <v>2.6447</v>
+        <v>2.7631</v>
       </c>
       <c r="AK24" t="s">
         <v>24</v>
       </c>
       <c r="AL24">
-        <v>3.00375</v>
+        <v>2.80802</v>
       </c>
       <c r="AM24">
-        <v>3.1598</v>
+        <v>3.015</v>
       </c>
       <c r="AQ24" t="s">
         <v>24</v>
       </c>
       <c r="AR24">
-        <v>2.97176</v>
+        <v>3.59138</v>
       </c>
       <c r="AS24">
-        <v>3.2047</v>
+        <v>3.8198</v>
       </c>
       <c r="AW24" t="s">
         <v>24</v>
       </c>
       <c r="AX24">
-        <v>3.82961</v>
+        <v>3.95694</v>
       </c>
       <c r="AY24">
-        <v>3.9578</v>
+        <v>4.1086</v>
       </c>
       <c r="BC24" t="s">
         <v>24</v>
       </c>
       <c r="BD24">
-        <v>4.29346</v>
+        <v>4.12313</v>
       </c>
       <c r="BE24">
-        <v>4.4272</v>
-      </c>
-    </row>
-    <row r="25" spans="1:57">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
+        <v>4.2683</v>
+      </c>
+    </row>
+    <row r="25" spans="7:57">
       <c r="G25" t="s">
         <v>25</v>
       </c>
       <c r="H25">
-        <v>0.431</v>
+        <v>0.33397</v>
       </c>
       <c r="I25">
-        <v>0.668</v>
+        <v>0.5738</v>
       </c>
       <c r="M25" t="s">
         <v>25</v>
       </c>
       <c r="N25">
-        <v>1.03068</v>
+        <v>0.71389</v>
       </c>
       <c r="O25">
-        <v>1.2738</v>
+        <v>0.9426</v>
       </c>
       <c r="S25" t="s">
         <v>25</v>
       </c>
       <c r="T25">
-        <v>1.6154</v>
+        <v>1.02758</v>
       </c>
       <c r="U25">
-        <v>1.8261</v>
+        <v>1.2434</v>
       </c>
       <c r="Y25" t="s">
         <v>25</v>
       </c>
       <c r="Z25">
-        <v>1.75848</v>
+        <v>1.8905</v>
       </c>
       <c r="AA25">
-        <v>2.0045</v>
+        <v>2.0941</v>
       </c>
       <c r="AE25" t="s">
         <v>25</v>
       </c>
       <c r="AF25">
-        <v>2.49966</v>
+        <v>2.54233</v>
       </c>
       <c r="AG25">
-        <v>2.6889</v>
+        <v>2.7333</v>
       </c>
       <c r="AK25" t="s">
         <v>25</v>
       </c>
       <c r="AL25">
-        <v>2.84698</v>
+        <v>3.07943</v>
       </c>
       <c r="AM25">
-        <v>3.0057</v>
+        <v>3.269</v>
       </c>
       <c r="AQ25" t="s">
         <v>25</v>
       </c>
       <c r="AR25">
-        <v>3.18447</v>
+        <v>3.19964</v>
       </c>
       <c r="AS25">
-        <v>3.4171</v>
+        <v>3.3745</v>
       </c>
       <c r="AW25" t="s">
         <v>25</v>
       </c>
       <c r="AX25">
-        <v>3.89309</v>
+        <v>4.43834</v>
       </c>
       <c r="AY25">
-        <v>3.9986</v>
+        <v>4.5922</v>
       </c>
       <c r="BC25" t="s">
         <v>25</v>
       </c>
       <c r="BD25">
-        <v>4.71309</v>
+        <v>4.18691</v>
       </c>
       <c r="BE25">
-        <v>4.8421</v>
-      </c>
-    </row>
-    <row r="26" spans="1:57">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
+        <v>4.3441</v>
+      </c>
+    </row>
+    <row r="26" spans="7:57">
       <c r="G26" t="s">
         <v>26</v>
       </c>
       <c r="H26">
-        <v>0.4152</v>
+        <v>0.34848</v>
       </c>
       <c r="I26">
-        <v>0.6535</v>
+        <v>0.5917</v>
       </c>
       <c r="M26" t="s">
         <v>26</v>
       </c>
       <c r="N26">
-        <v>1.2481</v>
+        <v>0.65045</v>
       </c>
       <c r="O26">
-        <v>1.4968</v>
+        <v>0.8784</v>
       </c>
       <c r="S26" t="s">
         <v>26</v>
       </c>
       <c r="T26">
-        <v>1.67066</v>
+        <v>1.07423</v>
       </c>
       <c r="U26">
-        <v>1.8819</v>
+        <v>1.3209</v>
       </c>
       <c r="Y26" t="s">
         <v>26</v>
       </c>
       <c r="Z26">
-        <v>1.81041</v>
+        <v>1.85772</v>
       </c>
       <c r="AA26">
-        <v>2.0094</v>
+        <v>2.0609</v>
       </c>
       <c r="AE26" t="s">
         <v>26</v>
       </c>
       <c r="AF26">
-        <v>2.46609</v>
+        <v>2.47336</v>
       </c>
       <c r="AG26">
-        <v>2.6493</v>
+        <v>2.6687</v>
       </c>
       <c r="AK26" t="s">
         <v>26</v>
       </c>
       <c r="AL26">
-        <v>2.77168</v>
+        <v>2.78084</v>
       </c>
       <c r="AM26">
-        <v>2.9427</v>
+        <v>2.971</v>
       </c>
       <c r="AQ26" t="s">
         <v>26</v>
       </c>
       <c r="AR26">
-        <v>2.87995</v>
+        <v>3.30174</v>
       </c>
       <c r="AS26">
-        <v>3.1119</v>
+        <v>3.4791</v>
       </c>
       <c r="AW26" t="s">
         <v>26</v>
       </c>
       <c r="AX26">
-        <v>4.13645</v>
+        <v>3.92206</v>
       </c>
       <c r="AY26">
-        <v>4.2812</v>
+        <v>4.0995</v>
       </c>
       <c r="BC26" t="s">
         <v>26</v>
       </c>
       <c r="BD26">
-        <v>6.8425</v>
+        <v>4.31819</v>
       </c>
       <c r="BE26">
-        <v>6.9791</v>
-      </c>
-    </row>
-    <row r="27" spans="1:57">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
+        <v>4.4637</v>
+      </c>
+    </row>
+    <row r="27" spans="7:57">
       <c r="G27" t="s">
         <v>27</v>
       </c>
       <c r="H27">
-        <v>0.43771</v>
+        <v>0.35571</v>
       </c>
       <c r="I27">
-        <v>0.6761</v>
+        <v>0.5982</v>
       </c>
       <c r="M27" t="s">
         <v>27</v>
       </c>
       <c r="N27">
-        <v>0.76863</v>
+        <v>0.70501</v>
       </c>
       <c r="O27">
-        <v>0.9925</v>
+        <v>0.9556</v>
       </c>
       <c r="S27" t="s">
         <v>27</v>
       </c>
       <c r="T27">
-        <v>1.23323</v>
+        <v>1.21712</v>
       </c>
       <c r="U27">
-        <v>1.4432</v>
+        <v>1.4366</v>
       </c>
       <c r="Y27" t="s">
         <v>27</v>
       </c>
       <c r="Z27">
-        <v>2.03</v>
+        <v>1.98872</v>
       </c>
       <c r="AA27">
-        <v>2.2283</v>
+        <v>2.1893</v>
       </c>
       <c r="AE27" t="s">
         <v>27</v>
       </c>
       <c r="AF27">
-        <v>2.75115</v>
+        <v>2.49192</v>
       </c>
       <c r="AG27">
-        <v>2.9301</v>
+        <v>2.6838</v>
       </c>
       <c r="AK27" t="s">
         <v>27</v>
       </c>
       <c r="AL27">
-        <v>2.87428</v>
+        <v>4.82867</v>
       </c>
       <c r="AM27">
-        <v>3.1042</v>
+        <v>5.068</v>
       </c>
       <c r="AQ27" t="s">
         <v>27</v>
       </c>
       <c r="AR27">
-        <v>3.12707</v>
+        <v>3.2846</v>
       </c>
       <c r="AS27">
-        <v>3.2919</v>
+        <v>3.4452</v>
       </c>
       <c r="AW27" t="s">
         <v>27</v>
       </c>
       <c r="AX27">
-        <v>5.10206</v>
+        <v>3.87075</v>
       </c>
       <c r="AY27">
-        <v>5.2446</v>
+        <v>4.0487</v>
       </c>
       <c r="BC27" t="s">
         <v>27</v>
       </c>
       <c r="BD27">
-        <v>4.46675</v>
+        <v>4.18359</v>
       </c>
       <c r="BE27">
-        <v>4.6008</v>
-      </c>
-    </row>
-    <row r="28" spans="1:57">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
+        <v>4.4177</v>
+      </c>
+    </row>
+    <row r="28" spans="7:57">
       <c r="G28" t="s">
         <v>28</v>
       </c>
       <c r="H28">
-        <v>0.57254</v>
+        <v>0.3592</v>
       </c>
       <c r="I28">
-        <v>0.8265</v>
+        <v>0.6014</v>
       </c>
       <c r="M28" t="s">
         <v>28</v>
       </c>
       <c r="N28">
-        <v>0.85246</v>
+        <v>0.65865</v>
       </c>
       <c r="O28">
-        <v>1.1004</v>
+        <v>0.8903</v>
       </c>
       <c r="S28" t="s">
         <v>28</v>
       </c>
       <c r="T28">
-        <v>1.23769</v>
+        <v>1.69196</v>
       </c>
       <c r="U28">
-        <v>1.4486</v>
+        <v>1.911</v>
       </c>
       <c r="Y28" t="s">
         <v>28</v>
       </c>
       <c r="Z28">
-        <v>1.97449</v>
+        <v>1.89863</v>
       </c>
       <c r="AA28">
-        <v>2.2178</v>
+        <v>2.0978</v>
       </c>
       <c r="AE28" t="s">
         <v>28</v>
       </c>
       <c r="AF28">
-        <v>2.42667</v>
+        <v>2.52504</v>
       </c>
       <c r="AG28">
-        <v>2.6602</v>
+        <v>2.7605</v>
       </c>
       <c r="AK28" t="s">
         <v>28</v>
       </c>
       <c r="AL28">
-        <v>2.85752</v>
+        <v>2.91329</v>
       </c>
       <c r="AM28">
-        <v>3.0346</v>
+        <v>3.1412</v>
       </c>
       <c r="AQ28" t="s">
         <v>28</v>
       </c>
       <c r="AR28">
-        <v>3.03244</v>
+        <v>3.58226</v>
       </c>
       <c r="AS28">
-        <v>3.197</v>
+        <v>3.7625</v>
       </c>
       <c r="AW28" t="s">
         <v>28</v>
       </c>
       <c r="AX28">
-        <v>4.17184</v>
+        <v>4.05672</v>
       </c>
       <c r="AY28">
-        <v>4.3306</v>
+        <v>4.2295</v>
       </c>
       <c r="BC28" t="s">
         <v>28</v>
       </c>
       <c r="BD28">
-        <v>4.41728</v>
+        <v>4.61533</v>
       </c>
       <c r="BE28">
-        <v>4.5459</v>
-      </c>
-    </row>
-    <row r="29" spans="1:57">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
+        <v>4.838</v>
+      </c>
+    </row>
+    <row r="29" spans="7:57">
       <c r="G29" t="s">
         <v>29</v>
       </c>
       <c r="H29">
-        <v>0.5254</v>
+        <v>0.3641</v>
       </c>
       <c r="I29">
-        <v>0.7619</v>
+        <v>0.6108</v>
       </c>
       <c r="M29" t="s">
         <v>29</v>
       </c>
       <c r="N29">
-        <v>0.8319</v>
+        <v>0.7452</v>
       </c>
       <c r="O29">
-        <v>1.0606</v>
+        <v>0.9774</v>
       </c>
       <c r="S29" t="s">
         <v>29</v>
       </c>
       <c r="T29">
-        <v>1.3633</v>
+        <v>1.1789</v>
       </c>
       <c r="U29">
-        <v>1.572</v>
+        <v>1.4004</v>
       </c>
       <c r="Y29" t="s">
         <v>29</v>
       </c>
       <c r="Z29">
-        <v>2.0057</v>
+        <v>2.002</v>
       </c>
       <c r="AA29">
-        <v>2.2193</v>
+        <v>2.2156</v>
       </c>
       <c r="AE29" t="s">
         <v>29</v>
       </c>
       <c r="AF29">
-        <v>2.4583</v>
+        <v>2.746</v>
       </c>
       <c r="AG29">
-        <v>2.6462</v>
+        <v>2.9494</v>
       </c>
       <c r="AK29" t="s">
         <v>29</v>
       </c>
       <c r="AL29">
-        <v>3.1168</v>
+        <v>3.0656</v>
       </c>
       <c r="AM29">
-        <v>3.2888</v>
+        <v>3.2575</v>
       </c>
       <c r="AQ29" t="s">
         <v>29</v>
       </c>
       <c r="AR29">
-        <v>3.3923</v>
+        <v>3.6089</v>
       </c>
       <c r="AS29">
-        <v>3.5652</v>
+        <v>3.7979</v>
       </c>
       <c r="AW29" t="s">
         <v>29</v>
       </c>
       <c r="AX29">
-        <v>4.1685</v>
+        <v>4.3761</v>
       </c>
       <c r="AY29">
-        <v>4.3211</v>
+        <v>4.5484</v>
       </c>
       <c r="BC29" t="s">
         <v>29</v>
       </c>
       <c r="BD29">
-        <v>5.7155</v>
+        <v>4.6296</v>
       </c>
       <c r="BE29">
-        <v>5.8265</v>
-      </c>
-    </row>
-    <row r="30" spans="1:57">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>1.1949</v>
-      </c>
+        <v>4.7907</v>
+      </c>
+    </row>
+    <row r="30" spans="7:57">
       <c r="G30" t="s">
         <v>30</v>
       </c>
       <c r="H30">
-        <v>10.0382</v>
+        <v>10.2127</v>
       </c>
       <c r="M30" t="s">
         <v>30</v>
       </c>
       <c r="N30">
-        <v>4.5062</v>
+        <v>4.3854</v>
       </c>
       <c r="S30" t="s">
         <v>30</v>
       </c>
       <c r="T30">
-        <v>4.0483</v>
+        <v>3.9608</v>
       </c>
       <c r="Y30" t="s">
         <v>30</v>
       </c>
       <c r="Z30">
-        <v>3.9492</v>
+        <v>3.8646</v>
       </c>
       <c r="AE30" t="s">
         <v>30</v>
       </c>
       <c r="AF30">
-        <v>3.9506</v>
+        <v>3.8658</v>
       </c>
       <c r="AK30" t="s">
         <v>30</v>
       </c>
       <c r="AL30">
-        <v>3.9515</v>
+        <v>3.8668</v>
       </c>
       <c r="AQ30" t="s">
         <v>30</v>
       </c>
       <c r="AR30">
-        <v>3.9515</v>
+        <v>3.8669</v>
       </c>
       <c r="AW30" t="s">
         <v>30</v>
       </c>
       <c r="AX30">
-        <v>3.9515</v>
+        <v>3.8669</v>
       </c>
       <c r="BC30" t="s">
         <v>30</v>
       </c>
       <c r="BD30">
-        <v>3.9515</v>
-      </c>
-    </row>
-    <row r="31" spans="1:57">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
+        <v>3.8669</v>
+      </c>
+    </row>
+    <row r="31" spans="7:57">
       <c r="G31" t="s">
         <v>31</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>0.0703</v>
       </c>
       <c r="M31" t="s">
         <v>31</v>
       </c>
       <c r="N31">
-        <v>0</v>
+        <v>0.0468</v>
       </c>
       <c r="S31" t="s">
         <v>31</v>
       </c>
       <c r="T31">
-        <v>0</v>
+        <v>0.0525</v>
       </c>
       <c r="Y31" t="s">
         <v>31</v>
       </c>
       <c r="Z31">
-        <v>0</v>
+        <v>0.0505</v>
       </c>
       <c r="AE31" t="s">
         <v>31</v>
       </c>
       <c r="AF31">
-        <v>0</v>
+        <v>0.0504</v>
       </c>
       <c r="AK31" t="s">
         <v>31</v>
       </c>
       <c r="AL31">
-        <v>0</v>
+        <v>0.0504</v>
       </c>
       <c r="AQ31" t="s">
         <v>31</v>
       </c>
       <c r="AR31">
-        <v>0</v>
+        <v>0.0504</v>
       </c>
       <c r="AW31" t="s">
         <v>31</v>
       </c>
       <c r="AX31">
-        <v>0</v>
+        <v>0.0504</v>
       </c>
       <c r="BC31" t="s">
         <v>31</v>
       </c>
       <c r="BD31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:57">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
+        <v>0.0504</v>
+      </c>
+    </row>
+    <row r="32" spans="7:57">
       <c r="G32" t="s">
         <v>32</v>
       </c>
       <c r="H32">
-        <v>0.0003</v>
+        <v>70.6541</v>
       </c>
       <c r="M32" t="s">
         <v>32</v>
       </c>
       <c r="N32">
-        <v>0.0002</v>
+        <v>35.3934</v>
       </c>
       <c r="S32" t="s">
         <v>32</v>
       </c>
       <c r="T32">
-        <v>0.0002</v>
+        <v>39.294</v>
       </c>
       <c r="Y32" t="s">
         <v>32</v>
       </c>
       <c r="Z32">
-        <v>0.0002</v>
+        <v>37.6799</v>
       </c>
       <c r="AE32" t="s">
         <v>32</v>
       </c>
       <c r="AF32">
-        <v>0.0002</v>
+        <v>37.6173</v>
       </c>
       <c r="AK32" t="s">
         <v>32</v>
       </c>
       <c r="AL32">
-        <v>0.0002</v>
+        <v>37.6461</v>
       </c>
       <c r="AQ32" t="s">
         <v>32</v>
       </c>
       <c r="AR32">
-        <v>0.0002</v>
+        <v>37.6491</v>
       </c>
       <c r="AW32" t="s">
         <v>32</v>
       </c>
       <c r="AX32">
-        <v>0.0002</v>
+        <v>37.6561</v>
       </c>
       <c r="BC32" t="s">
         <v>32</v>
       </c>
       <c r="BD32">
-        <v>0.0002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:56">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33">
-        <v>1.1949</v>
-      </c>
+        <v>37.6621</v>
+      </c>
+    </row>
+    <row r="33" spans="7:56">
       <c r="G33" t="s">
         <v>33</v>
       </c>
       <c r="H33">
-        <v>10.0382</v>
+        <v>10.283</v>
       </c>
       <c r="M33" t="s">
         <v>33</v>
       </c>
       <c r="N33">
-        <v>4.5062</v>
+        <v>4.4322</v>
       </c>
       <c r="S33" t="s">
         <v>33</v>
       </c>
       <c r="T33">
-        <v>4.0483</v>
+        <v>4.0133</v>
       </c>
       <c r="Y33" t="s">
         <v>33</v>
       </c>
       <c r="Z33">
-        <v>3.9492</v>
+        <v>3.9151</v>
       </c>
       <c r="AE33" t="s">
         <v>33</v>
       </c>
       <c r="AF33">
-        <v>3.9506</v>
+        <v>3.9162</v>
       </c>
       <c r="AK33" t="s">
         <v>33</v>
       </c>
       <c r="AL33">
-        <v>3.9515</v>
+        <v>3.9172</v>
       </c>
       <c r="AQ33" t="s">
         <v>33</v>
       </c>
       <c r="AR33">
-        <v>3.9515</v>
+        <v>3.9173</v>
       </c>
       <c r="AW33" t="s">
         <v>33</v>
       </c>
       <c r="AX33">
-        <v>3.9515</v>
+        <v>3.9173</v>
       </c>
       <c r="BC33" t="s">
         <v>33</v>
       </c>
       <c r="BD33">
-        <v>3.9515</v>
-      </c>
-    </row>
-    <row r="34" spans="1:56">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <v>1.1949</v>
-      </c>
+        <v>3.9173</v>
+      </c>
+    </row>
+    <row r="34" spans="7:56">
       <c r="G34" t="s">
         <v>34</v>
       </c>
       <c r="H34">
-        <v>10.0385</v>
+        <v>80.8668</v>
       </c>
       <c r="M34" t="s">
         <v>34</v>
       </c>
       <c r="N34">
-        <v>4.5064</v>
+        <v>39.7788</v>
       </c>
       <c r="S34" t="s">
         <v>34</v>
       </c>
       <c r="T34">
-        <v>4.048500000000001</v>
+        <v>43.2548</v>
       </c>
       <c r="Y34" t="s">
         <v>34</v>
       </c>
       <c r="Z34">
-        <v>3.9494</v>
+        <v>41.54450000000001</v>
       </c>
       <c r="AE34" t="s">
         <v>34</v>
       </c>
       <c r="AF34">
-        <v>3.9508</v>
+        <v>41.4831</v>
       </c>
       <c r="AK34" t="s">
         <v>34</v>
       </c>
       <c r="AL34">
-        <v>3.9517</v>
+        <v>41.51289999999999</v>
       </c>
       <c r="AQ34" t="s">
         <v>34</v>
       </c>
       <c r="AR34">
-        <v>3.9517</v>
+        <v>41.516</v>
       </c>
       <c r="AW34" t="s">
         <v>34</v>
       </c>
       <c r="AX34">
-        <v>3.9517</v>
+        <v>41.523</v>
       </c>
       <c r="BC34" t="s">
         <v>34</v>
       </c>
       <c r="BD34">
-        <v>3.9517</v>
-      </c>
-    </row>
-    <row r="35" spans="1:56">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35">
-        <v>1.1949</v>
-      </c>
+        <v>41.529</v>
+      </c>
+    </row>
+    <row r="35" spans="7:56">
       <c r="G35" t="s">
         <v>35</v>
       </c>
       <c r="H35">
-        <v>10.0385</v>
+        <v>80.9371</v>
       </c>
       <c r="M35" t="s">
         <v>35</v>
       </c>
       <c r="N35">
-        <v>4.5064</v>
+        <v>39.8256</v>
       </c>
       <c r="S35" t="s">
         <v>35</v>
       </c>
       <c r="T35">
-        <v>4.048500000000001</v>
+        <v>43.3073</v>
       </c>
       <c r="Y35" t="s">
         <v>35</v>
       </c>
       <c r="Z35">
-        <v>3.9494</v>
+        <v>41.59500000000001</v>
       </c>
       <c r="AE35" t="s">
         <v>35</v>
       </c>
       <c r="AF35">
-        <v>3.9508</v>
+        <v>41.5335</v>
       </c>
       <c r="AK35" t="s">
         <v>35</v>
       </c>
       <c r="AL35">
-        <v>3.9517</v>
+        <v>41.5633</v>
       </c>
       <c r="AQ35" t="s">
         <v>35</v>
       </c>
       <c r="AR35">
-        <v>3.9517</v>
+        <v>41.56639999999999</v>
       </c>
       <c r="AW35" t="s">
         <v>35</v>
       </c>
       <c r="AX35">
-        <v>3.9517</v>
+        <v>41.5734</v>
       </c>
       <c r="BC35" t="s">
         <v>35</v>
       </c>
       <c r="BD35">
-        <v>3.9517</v>
-      </c>
-    </row>
-    <row r="36" spans="1:56">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36">
-        <v>3519.5443</v>
-      </c>
+        <v>41.5794</v>
+      </c>
+    </row>
+    <row r="36" spans="7:56">
       <c r="G36" t="s">
         <v>36</v>
       </c>
       <c r="H36">
-        <v>1282.8017</v>
+        <v>1282.629</v>
       </c>
       <c r="M36" t="s">
         <v>36</v>
       </c>
       <c r="N36">
-        <v>1304.5566</v>
+        <v>1304.4294</v>
       </c>
       <c r="S36" t="s">
         <v>36</v>
       </c>
       <c r="T36">
-        <v>1300.0003</v>
+        <v>1299.98</v>
       </c>
       <c r="Y36" t="s">
         <v>36</v>
       </c>
       <c r="Z36">
-        <v>1298.5812</v>
+        <v>1298.5539</v>
       </c>
       <c r="AE36" t="s">
         <v>36</v>
       </c>
       <c r="AF36">
-        <v>1298.598</v>
+        <v>1298.5683</v>
       </c>
       <c r="AK36" t="s">
         <v>36</v>
       </c>
       <c r="AL36">
-        <v>1298.6235</v>
+        <v>1298.5953</v>
       </c>
       <c r="AQ36" t="s">
         <v>36</v>
       </c>
       <c r="AR36">
-        <v>1298.6246</v>
+        <v>1298.5967</v>
       </c>
       <c r="AW36" t="s">
         <v>36</v>
       </c>
       <c r="AX36">
-        <v>1298.6242</v>
+        <v>1298.5963</v>
       </c>
       <c r="BC36" t="s">
         <v>36</v>
       </c>
       <c r="BD36">
-        <v>1298.6242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:56">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37">
-        <v>3519.5443</v>
-      </c>
+        <v>1298.5962</v>
+      </c>
+    </row>
+    <row r="37" spans="7:56">
       <c r="G37" t="s">
         <v>37</v>
       </c>
       <c r="H37">
-        <v>1282.8017</v>
+        <v>1282.629</v>
       </c>
       <c r="M37" t="s">
         <v>37</v>
       </c>
       <c r="N37">
-        <v>1304.5566</v>
+        <v>1304.4294</v>
       </c>
       <c r="S37" t="s">
         <v>37</v>
       </c>
       <c r="T37">
-        <v>1300.0003</v>
+        <v>1299.98</v>
       </c>
       <c r="Y37" t="s">
         <v>37</v>
       </c>
       <c r="Z37">
-        <v>1298.5812</v>
+        <v>1298.5539</v>
       </c>
       <c r="AE37" t="s">
         <v>37</v>
       </c>
       <c r="AF37">
-        <v>1298.598</v>
+        <v>1298.5683</v>
       </c>
       <c r="AK37" t="s">
         <v>37</v>
       </c>
       <c r="AL37">
-        <v>1298.6235</v>
+        <v>1298.5953</v>
       </c>
       <c r="AQ37" t="s">
         <v>37</v>
       </c>
       <c r="AR37">
-        <v>1298.6246</v>
+        <v>1298.5967</v>
       </c>
       <c r="AW37" t="s">
         <v>37</v>
       </c>
       <c r="AX37">
-        <v>1298.6242</v>
+        <v>1298.5963</v>
       </c>
       <c r="BC37" t="s">
         <v>37</v>
       </c>
       <c r="BD37">
-        <v>1298.6242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:56">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38">
-        <v>1.2462</v>
-      </c>
+        <v>1298.5962</v>
+      </c>
+    </row>
+    <row r="38" spans="7:56">
       <c r="G38" t="s">
         <v>38</v>
       </c>
       <c r="H38">
-        <v>8.6843</v>
+        <v>8.684900000000001</v>
       </c>
       <c r="M38" t="s">
         <v>38</v>
       </c>
       <c r="N38">
-        <v>8.588699999999999</v>
+        <v>8.5893</v>
       </c>
       <c r="S38" t="s">
         <v>38</v>
       </c>
       <c r="T38">
-        <v>8.6089</v>
+        <v>8.609</v>
       </c>
       <c r="Y38" t="s">
         <v>38</v>
       </c>
       <c r="Z38">
-        <v>8.6151</v>
+        <v>8.6153</v>
       </c>
       <c r="AE38" t="s">
         <v>38</v>
       </c>
       <c r="AF38">
-        <v>8.6151</v>
+        <v>8.6152</v>
       </c>
       <c r="AK38" t="s">
         <v>38</v>
       </c>
       <c r="AL38">
-        <v>8.615</v>
+        <v>8.6151</v>
       </c>
       <c r="AQ38" t="s">
         <v>38</v>
       </c>
       <c r="AR38">
-        <v>8.615</v>
+        <v>8.6151</v>
       </c>
       <c r="AW38" t="s">
         <v>38</v>
       </c>
       <c r="AX38">
-        <v>8.615</v>
+        <v>8.6151</v>
       </c>
       <c r="BC38" t="s">
         <v>38</v>
       </c>
       <c r="BD38">
-        <v>8.615</v>
-      </c>
-    </row>
-    <row r="39" spans="1:56">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39">
-        <v>0.0002</v>
-      </c>
+        <v>8.6151</v>
+      </c>
+    </row>
+    <row r="39" spans="7:56">
       <c r="G39" t="s">
         <v>39</v>
       </c>
       <c r="H39">
-        <v>0.0173</v>
+        <v>0.0175</v>
       </c>
       <c r="M39" t="s">
         <v>39</v>
       </c>
       <c r="N39">
-        <v>0.0316</v>
+        <v>0.0315</v>
       </c>
       <c r="S39" t="s">
         <v>39</v>
       </c>
       <c r="T39">
-        <v>0.0259</v>
+        <v>0.026</v>
       </c>
       <c r="Y39" t="s">
         <v>39</v>
       </c>
       <c r="Z39">
-        <v>0.0247</v>
+        <v>0.0248</v>
       </c>
       <c r="AE39" t="s">
         <v>39</v>
       </c>
       <c r="AF39">
-        <v>0.0248</v>
+        <v>0.0249</v>
       </c>
       <c r="AK39" t="s">
         <v>39</v>
       </c>
       <c r="AL39">
-        <v>0.0248</v>
+        <v>0.0249</v>
       </c>
       <c r="AQ39" t="s">
         <v>39</v>
       </c>
       <c r="AR39">
-        <v>0.0248</v>
+        <v>0.0249</v>
       </c>
       <c r="AW39" t="s">
         <v>39</v>
       </c>
       <c r="AX39">
-        <v>0.0248</v>
+        <v>0.0249</v>
       </c>
       <c r="BC39" t="s">
         <v>39</v>
       </c>
       <c r="BD39">
-        <v>0.0248</v>
-      </c>
-    </row>
-    <row r="40" spans="1:56">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40">
-        <v>0.8</v>
-      </c>
+        <v>0.0249</v>
+      </c>
+    </row>
+    <row r="40" spans="7:56">
       <c r="G40" t="s">
         <v>40</v>
       </c>
       <c r="H40">
-        <v>0.7984</v>
+        <v>0.7982</v>
       </c>
       <c r="M40" t="s">
         <v>40</v>
@@ -3528,31 +3357,31 @@
         <v>40</v>
       </c>
       <c r="AF40">
-        <v>0.7993</v>
+        <v>0.7992</v>
       </c>
       <c r="AK40" t="s">
         <v>40</v>
       </c>
       <c r="AL40">
-        <v>0.7993</v>
+        <v>0.7992</v>
       </c>
       <c r="AQ40" t="s">
         <v>40</v>
       </c>
       <c r="AR40">
-        <v>0.7993</v>
+        <v>0.7992</v>
       </c>
       <c r="AW40" t="s">
         <v>40</v>
       </c>
       <c r="AX40">
-        <v>0.7993</v>
+        <v>0.7992</v>
       </c>
       <c r="BC40" t="s">
         <v>40</v>
       </c>
       <c r="BD40">
-        <v>0.7993</v>
+        <v>0.7992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>